<commit_message>
limit only _DIR can be set as parent
</commit_message>
<xml_diff>
--- a/folder-sample.xlsx
+++ b/folder-sample.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="104">
   <si>
     <t>標題</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -91,22 +91,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>DIR</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>業務相關</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>這裡的資料跟業務有關</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>業務,客戶</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>parent</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -186,10 +170,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>銷售 DM</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>相關的 DM 都在這邊喔!</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -198,14 +178,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>銷售中的 - 104年電聯車維修授證班</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R:\folder\1.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>R:\folder\2.png</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -222,12 +194,194 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>PowerCam 軟體教學與展示 - PowerCam Media</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>PowerCam 軟體教學與展示 - PowerCam Media</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>銷售 DM - 1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>銷售 DM - 2</t>
+  </si>
+  <si>
+    <t>銷售 DM - 3</t>
+  </si>
+  <si>
+    <t>銷售 DM - 4</t>
+  </si>
+  <si>
+    <t>銷售 DM - 5</t>
+  </si>
+  <si>
+    <t>銷售 DM - 6</t>
+  </si>
+  <si>
+    <t>銷售 DM - 7</t>
+  </si>
+  <si>
+    <t>銷售 DM - 8</t>
+  </si>
+  <si>
+    <t>銷售 DM - 9</t>
+  </si>
+  <si>
+    <t>銷售 DM - 10</t>
+  </si>
+  <si>
+    <t>銷售 DM - 11</t>
+  </si>
+  <si>
+    <t>銷售 DM - 12</t>
+  </si>
+  <si>
+    <t>銷售 DM - 13</t>
+  </si>
+  <si>
+    <t>銷售 DM - 14</t>
+  </si>
+  <si>
+    <t>R:\folder\4.jpeg</t>
+  </si>
+  <si>
+    <t>admin:ben02admin</t>
+  </si>
+  <si>
+    <t>105年票務系統操作人員授證訓練班(1):資料夾管理者2</t>
+  </si>
+  <si>
+    <t>2|資料夾管理者5:助理管理師</t>
+  </si>
+  <si>
+    <t>R:\folder\5.jpeg</t>
+  </si>
+  <si>
+    <t>admin:ben03admin</t>
+  </si>
+  <si>
+    <t>105年票務系統操作人員授證訓練班(1):資料夾管理者3</t>
+  </si>
+  <si>
+    <t>2|資料夾管理者6:助理管理師</t>
+  </si>
+  <si>
+    <t>R:\folder\6.jpeg</t>
+  </si>
+  <si>
+    <t>admin:ben04admin</t>
+  </si>
+  <si>
+    <t>105年票務系統操作人員授證訓練班(1):資料夾管理者4</t>
+  </si>
+  <si>
+    <t>2|資料夾管理者7:助理管理師</t>
+  </si>
+  <si>
+    <t>R:\folder\7.jpeg</t>
+  </si>
+  <si>
+    <t>admin:ben05admin</t>
+  </si>
+  <si>
+    <t>105年票務系統操作人員授證訓練班(1):資料夾管理者5</t>
+  </si>
+  <si>
+    <t>2|資料夾管理者8:助理管理師</t>
+  </si>
+  <si>
+    <t>R:\folder\8.jpeg</t>
+  </si>
+  <si>
+    <t>admin:ben06admin</t>
+  </si>
+  <si>
+    <t>105年票務系統操作人員授證訓練班(1):資料夾管理者6</t>
+  </si>
+  <si>
+    <t>2|資料夾管理者9:助理管理師</t>
+  </si>
+  <si>
+    <t>R:\folder\9.jpeg</t>
+  </si>
+  <si>
+    <t>admin:ben07admin</t>
+  </si>
+  <si>
+    <t>105年票務系統操作人員授證訓練班(1):資料夾管理者7</t>
+  </si>
+  <si>
+    <t>2|資料夾管理者10:助理管理師</t>
+  </si>
+  <si>
+    <t>R:\folder\10.jpeg</t>
+  </si>
+  <si>
+    <t>admin:ben08admin</t>
+  </si>
+  <si>
+    <t>105年票務系統操作人員授證訓練班(1):資料夾管理者8</t>
+  </si>
+  <si>
+    <t>2|資料夾管理者11:助理管理師</t>
+  </si>
+  <si>
+    <t>R:\folder\11.jpeg</t>
+  </si>
+  <si>
+    <t>admin:ben09admin</t>
+  </si>
+  <si>
+    <t>105年票務系統操作人員授證訓練班(1):資料夾管理者9</t>
+  </si>
+  <si>
+    <t>2|資料夾管理者12:助理管理師</t>
+  </si>
+  <si>
+    <t>R:\folder\12.jpeg</t>
+  </si>
+  <si>
+    <t>admin:ben10admin</t>
+  </si>
+  <si>
+    <t>105年票務系統操作人員授證訓練班(1):資料夾管理者10</t>
+  </si>
+  <si>
+    <t>2|資料夾管理者13:助理管理師</t>
+  </si>
+  <si>
+    <t>R:\folder\13.jpeg</t>
+  </si>
+  <si>
+    <t>admin:ben11admin</t>
+  </si>
+  <si>
+    <t>105年票務系統操作人員授證訓練班(1):資料夾管理者11</t>
+  </si>
+  <si>
+    <t>2|資料夾管理者14:助理管理師</t>
+  </si>
+  <si>
+    <t>R:\folder\14.jpeg</t>
+  </si>
+  <si>
+    <t>admin:ben12admin</t>
+  </si>
+  <si>
+    <t>105年票務系統操作人員授證訓練班(1):資料夾管理者12</t>
+  </si>
+  <si>
+    <t>2|資料夾管理者15:助理管理師</t>
+  </si>
+  <si>
+    <t>R:\folder\15.jpeg</t>
+  </si>
+  <si>
+    <t>admin:ben13admin</t>
+  </si>
+  <si>
+    <t>105年票務系統操作人員授證訓練班(1):資料夾管理者13</t>
+  </si>
+  <si>
+    <t>2|資料夾管理者16:助理管理師</t>
+  </si>
+  <si>
+    <t>BBBBBBBB</t>
   </si>
 </sst>
 </file>
@@ -617,10 +771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -628,7 +782,7 @@
     <col min="1" max="1" width="26.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.625" customWidth="1"/>
+    <col min="4" max="4" width="35.5" customWidth="1"/>
     <col min="5" max="5" width="13.625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="5.5" bestFit="1" customWidth="1"/>
@@ -690,101 +844,122 @@
     </row>
     <row r="2" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="N2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="3" t="s">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="H3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="J3" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="O2" s="3" t="s">
+      <c r="K3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="L3">
+        <v>100</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
         <v>32</v>
       </c>
-      <c r="H3" t="s">
-        <v>43</v>
+      <c r="O3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>103</v>
       </c>
       <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" t="s">
         <v>38</v>
       </c>
-      <c r="D4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" t="s">
-        <v>44</v>
-      </c>
       <c r="I4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="K4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="L4">
         <v>100</v>
@@ -793,42 +968,39 @@
         <v>1</v>
       </c>
       <c r="N4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="O4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5">
-        <v>1164</v>
+        <v>103</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H5" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="I5" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="J5" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="K5" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="L5">
         <v>100</v>
@@ -837,10 +1009,461 @@
         <v>1</v>
       </c>
       <c r="N5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" t="s">
         <v>36</v>
       </c>
-      <c r="O5" t="s">
-        <v>37</v>
+      <c r="G6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" t="s">
+        <v>60</v>
+      </c>
+      <c r="J6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K6" t="s">
+        <v>62</v>
+      </c>
+      <c r="L6">
+        <v>100</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6" t="s">
+        <v>32</v>
+      </c>
+      <c r="O6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I7" t="s">
+        <v>64</v>
+      </c>
+      <c r="J7" t="s">
+        <v>65</v>
+      </c>
+      <c r="K7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L7">
+        <v>100</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7" t="s">
+        <v>32</v>
+      </c>
+      <c r="O7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" t="s">
+        <v>67</v>
+      </c>
+      <c r="I8" t="s">
+        <v>68</v>
+      </c>
+      <c r="J8" t="s">
+        <v>69</v>
+      </c>
+      <c r="K8" t="s">
+        <v>70</v>
+      </c>
+      <c r="L8">
+        <v>100</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8" t="s">
+        <v>32</v>
+      </c>
+      <c r="O8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" t="s">
+        <v>71</v>
+      </c>
+      <c r="I9" t="s">
+        <v>72</v>
+      </c>
+      <c r="J9" t="s">
+        <v>73</v>
+      </c>
+      <c r="K9" t="s">
+        <v>74</v>
+      </c>
+      <c r="L9">
+        <v>100</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9" t="s">
+        <v>32</v>
+      </c>
+      <c r="O9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" t="s">
+        <v>76</v>
+      </c>
+      <c r="J10" t="s">
+        <v>77</v>
+      </c>
+      <c r="K10" t="s">
+        <v>78</v>
+      </c>
+      <c r="L10">
+        <v>100</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10" t="s">
+        <v>32</v>
+      </c>
+      <c r="O10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" t="s">
+        <v>79</v>
+      </c>
+      <c r="I11" t="s">
+        <v>80</v>
+      </c>
+      <c r="J11" t="s">
+        <v>81</v>
+      </c>
+      <c r="K11" t="s">
+        <v>82</v>
+      </c>
+      <c r="L11">
+        <v>100</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11" t="s">
+        <v>32</v>
+      </c>
+      <c r="O11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" t="s">
+        <v>83</v>
+      </c>
+      <c r="I12" t="s">
+        <v>84</v>
+      </c>
+      <c r="J12" t="s">
+        <v>85</v>
+      </c>
+      <c r="K12" t="s">
+        <v>86</v>
+      </c>
+      <c r="L12">
+        <v>100</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12" t="s">
+        <v>32</v>
+      </c>
+      <c r="O12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" t="s">
+        <v>87</v>
+      </c>
+      <c r="I13" t="s">
+        <v>88</v>
+      </c>
+      <c r="J13" t="s">
+        <v>89</v>
+      </c>
+      <c r="K13" t="s">
+        <v>90</v>
+      </c>
+      <c r="L13">
+        <v>100</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13" t="s">
+        <v>32</v>
+      </c>
+      <c r="O13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" t="s">
+        <v>91</v>
+      </c>
+      <c r="I14" t="s">
+        <v>92</v>
+      </c>
+      <c r="J14" t="s">
+        <v>93</v>
+      </c>
+      <c r="K14" t="s">
+        <v>94</v>
+      </c>
+      <c r="L14">
+        <v>100</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14" t="s">
+        <v>32</v>
+      </c>
+      <c r="O14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" t="s">
+        <v>95</v>
+      </c>
+      <c r="I15" t="s">
+        <v>96</v>
+      </c>
+      <c r="J15" t="s">
+        <v>97</v>
+      </c>
+      <c r="K15" t="s">
+        <v>98</v>
+      </c>
+      <c r="L15">
+        <v>100</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15" t="s">
+        <v>32</v>
+      </c>
+      <c r="O15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" t="s">
+        <v>99</v>
+      </c>
+      <c r="I16" t="s">
+        <v>100</v>
+      </c>
+      <c r="J16" t="s">
+        <v>101</v>
+      </c>
+      <c r="K16" t="s">
+        <v>102</v>
+      </c>
+      <c r="L16">
+        <v>100</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16" t="s">
+        <v>32</v>
+      </c>
+      <c r="O16" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>